<commit_message>
Batch bugfix 1. Fixed Fwd Agent being replaced 2. Enabled CMA/ANL multiple transshipment 3. Changed saved files naming convention 4. Changed MSC to use today's date instead of first day of month 5. Added g2_whitespace_rows configuration
</commit_message>
<xml_diff>
--- a/data/Configurations.xlsx
+++ b/data/Configurations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tym.Teo\Rio Tinto\RTA Logistics - General\Scripts\Delay Report\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tym.Teo\Documents\Delay Report - Rewrite\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{88136CCA-AA4A-483E-823E-20CCE4D1CE3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BF160761-C705-4A22-BD52-039B77EDD208}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027ED4D5-D675-4406-83C0-BC62CF355108}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="66">
   <si>
     <t>Booking Office</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>run_one</t>
+  </si>
+  <si>
+    <t>g2_whitespace_rows</t>
   </si>
 </sst>
 </file>
@@ -692,11 +695,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -779,26 +782,26 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="9" t="b">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
+      </c>
+      <c r="B12" s="9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -831,6 +834,14 @@
       </c>
       <c r="B16" s="9" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="7">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1815,18 +1826,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2047,18 +2058,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE68490-0574-4399-8E76-2FC2ACED3CAE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01DD0693-FE4D-4885-BF24-94BEA9248921}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01DD0693-FE4D-4885-BF24-94BEA9248921}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE68490-0574-4399-8E76-2FC2ACED3CAE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Second batch bugfix 1. Changed ANL/CMA to get 6 weeks from today 2. Changed Hamburg to get 6 weeks from today 3. Changed all instances of first_day to today 4. Fixed COSCO transshipment
</commit_message>
<xml_diff>
--- a/data/Configurations.xlsx
+++ b/data/Configurations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tym.Teo\Documents\Delay Report - Rewrite\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027ED4D5-D675-4406-83C0-BC62CF355108}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FACF307-52B0-4957-87B7-4E1B3E36B6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -699,7 +699,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1826,21 +1826,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003B07C177EC98944892D6859FC7228F27" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fa0312146baf983fe551619124602045">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cadb0006-b086-403f-9c46-c0186d7f6965" xmlns:ns3="4af93f69-0cef-4f40-803d-f637351e1512" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c8aa75208339fe16869b5142f429bf55" ns2:_="" ns3:_="">
     <xsd:import namespace="cadb0006-b086-403f-9c46-c0186d7f6965"/>
@@ -2057,24 +2042,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01DD0693-FE4D-4885-BF24-94BEA9248921}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE68490-0574-4399-8E76-2FC2ACED3CAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80FBAC62-C129-4627-A795-495E3326B79B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2091,4 +2074,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE68490-0574-4399-8E76-2FC2ACED3CAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01DD0693-FE4D-4885-BF24-94BEA9248921}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed a bug with ONEExtractor at end of month, added debug_mode configuration
</commit_message>
<xml_diff>
--- a/data/Configurations.xlsx
+++ b/data/Configurations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tym.Teo\Documents\Delay Report - Rewrite\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FACF307-52B0-4957-87B7-4E1B3E36B6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F2DF48-DCB4-4BD1-95ED-976A1D5C179E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="67">
   <si>
     <t>Booking Office</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>g2_whitespace_rows</t>
+  </si>
+  <si>
+    <t>debug_mode</t>
   </si>
 </sst>
 </file>
@@ -695,11 +698,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -806,42 +809,50 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="7">
-        <v>2</v>
+        <v>66</v>
+      </c>
+      <c r="B13" s="9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="9" t="b">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="B15" s="7">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="9" t="b">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="B16" s="7">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="7">
-        <v>9</v>
+        <v>62</v>
+      </c>
+      <c r="B17" s="9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="9" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1826,6 +1837,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003B07C177EC98944892D6859FC7228F27" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fa0312146baf983fe551619124602045">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cadb0006-b086-403f-9c46-c0186d7f6965" xmlns:ns3="4af93f69-0cef-4f40-803d-f637351e1512" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c8aa75208339fe16869b5142f429bf55" ns2:_="" ns3:_="">
     <xsd:import namespace="cadb0006-b086-403f-9c46-c0186d7f6965"/>
@@ -2042,12 +2059,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2058,6 +2069,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE68490-0574-4399-8E76-2FC2ACED3CAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80FBAC62-C129-4627-A795-495E3326B79B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2076,15 +2096,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE68490-0574-4399-8E76-2FC2ACED3CAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01DD0693-FE4D-4885-BF24-94BEA9248921}">
   <ds:schemaRefs>

</xml_diff>